<commit_message>
x3 in plate constants
</commit_message>
<xml_diff>
--- a/backend/auxiliar/albireo.astropy-units.xlsx
+++ b/backend/auxiliar/albireo.astropy-units.xlsx
@@ -647,31 +647,31 @@
         <v>0</v>
       </c>
       <c r="Q2" t="n">
-        <v>292.9450616659929</v>
+        <v>292.9762230766974</v>
       </c>
       <c r="R2" t="n">
-        <v>27.9722122418775</v>
+        <v>28.03907201365526</v>
       </c>
       <c r="S2" t="inlineStr">
         <is>
-          <t>{'simbad': {'x': 0.8288716931606084, 'y': 0.46603169252647836, 'z': 0.3094934213161437, 'ar': 5.108235152768638, 'dec': 0.4879883626478569, 'ar_deg': 292.68031501400833, 'dec_deg': 27.959673631221666, 'pmra': 4.915, 'pmdec': -11.127}, 'proper motion': {'ar': 5.10823576494002, 'dec': 0.48798697676159847, 'pmra': 4.915, 'pmdec': -11.127}, 'precession': {'x': 0.3440880094260904, 'y': -0.8130081398518701, 'z': 0.4697033173225333, 'ar': 5.112757980058873, 'dec': 0.48895468712731205, 'ang_zeta': 0.0028852121230277415, 'ang_theta': 0.002496113304495591, 'ang_z': 0.0028597582311986106}, 'nutation': {'x': 0.3440979195634882, 'y': -0.8130242623062829, 'z': 0.4696681494985619, 'ar': 5.112761199835909, 'dec': 0.488914851963959, 'dpsi': 1.7724397752215108e-05, 'deps': 4.623967697805032e-05, 'epsm': 0.4090344953255741, 'w': -6.489953776770748}, 'aberration': {'x': 0.34413147418926954, 'y': -0.8129745387999108, 'z': 0.46972963259240114, 'ar': 5.112818155764926, 'dec': 0.4889844954116079, 'lambda_s': 2.9546338179558234, 'epsilon_m': 0.4090294332006951, 'omega_bar': 4.939647965644993}, 'refraction': {'x': 0.3443043576989555, 'y': -0.8132975486127773, 'z': 0.4690432887164638, 'ar': 5.112855853529401, 'dec': 0.4882072026874268, 'R': -160.47507890873985, 'alt': -20.500975505001563}}</t>
+          <t>{'simbad': {'x': 0.8288716931606084, 'y': 0.46603169252647836, 'z': 0.3094934213161437, 'ar': 5.108235152768638, 'dec': 0.4879883626478569, 'ar_deg': 292.68031501400833, 'dec_deg': 27.959673631221666, 'pmra': 4.915, 'pmdec': -11.127}, 'proper motion': {'ar': 5.108235765983847, 'dec': 0.48798697439849514, 'pmra': 4.915, 'pmdec': -11.127}, 'precession': {'x': 0.34409397639612477, 'y': -0.8130047695557148, 'z': 0.4697047797154744, 'ar': 5.112765692456297, 'dec': 0.4889563436217464, 'ang_zeta': 0.0028901100151612243, 'ang_theta': 0.002500369232447987, 'ang_z': 0.0028646569776294853}, 'nutation': {'x': 0.344102473026793, 'y': -0.8130214717747243, 'z': 0.4696696439946977, 'ar': 5.112767181649722, 'dec': 0.4889165447867427, 'dpsi': 1.519641027055965e-05, 'deps': 4.577484563030587e-05, 'epsm': 0.4090343959020549, 'w': -6.5047412493804675}, 'aberration': {'x': 0.34411228782423137, 'y': -0.8129787418679203, 'z': 0.469736414001753, 'ar': 5.112796285725964, 'dec': 0.48899217704265424, 'lambda_s': 3.229878486430863, 'epsilon_m': 0.40902933380891293, 'omega_bar': 4.939650435148504}, 'refraction': {'x': 0.34453274689249547, 'y': -0.8126057027934914, 'z': 0.4700735666959026, 'ar': 5.113399722745761, 'dec': 0.48937412584208084, 'R': 135.19646097722926, 'alt': 24.326828200962666}}</t>
         </is>
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>19h31m46.815s</t>
+          <t>19h31m54.294s</t>
         </is>
       </c>
       <c r="U2" t="inlineStr">
         <is>
-          <t>+27°58'19.964"</t>
+          <t>+28°02'20.659"</t>
         </is>
       </c>
       <c r="V2" t="n">
-        <v>5.112855853529401</v>
+        <v>5.113399722745761</v>
       </c>
       <c r="W2" t="n">
-        <v>0.4882072026874268</v>
+        <v>0.4893741258420808</v>
       </c>
       <c r="X2" t="inlineStr">
         <is>
@@ -691,25 +691,25 @@
       </c>
       <c r="AB2" t="inlineStr">
         <is>
-          <t>19h31m46.815s</t>
+          <t>19h31m54.294s</t>
         </is>
       </c>
       <c r="AC2" t="inlineStr">
         <is>
-          <t>+27°58'19.964"</t>
+          <t>+28°02'20.659"</t>
         </is>
       </c>
       <c r="AD2" t="n">
-        <v>5.112855853529401</v>
+        <v>5.113399722745761</v>
       </c>
       <c r="AE2" t="n">
-        <v>0.4882072026874268</v>
+        <v>0.4893741258420808</v>
       </c>
       <c r="AF2" t="n">
-        <v>-0.001564419154135521</v>
+        <v>292.9762449333871</v>
       </c>
       <c r="AG2" t="n">
-        <v>-0.001212261274563531</v>
+        <v>28.03899255004892</v>
       </c>
     </row>
     <row r="3">
@@ -764,31 +764,31 @@
         <v>1</v>
       </c>
       <c r="Q3" t="n">
-        <v>293.0782328833088</v>
+        <v>293.1093896976551</v>
       </c>
       <c r="R3" t="n">
-        <v>27.90845403061904</v>
+        <v>27.97510462551637</v>
       </c>
       <c r="S3" t="inlineStr">
         <is>
-          <t>{'simbad': {'x': 0.7422745682107805, 'y': 0.5587448361350019, 'z': 0.3699090070273623, 'ar': 5.110557462390437, 'dec': 0.4868669741583784, 'ar_deg': 292.81337355406, 'dec_deg': 27.895422803579997, 'pmra': -2.408, 'pmdec': -5.353}, 'proper motion': {'ar': 5.110557162470053, 'dec': 0.4868663074333724, 'pmra': -2.408, 'pmdec': -5.353}, 'precession': {'x': 0.34618313384554456, 'y': -0.812687092143297, 'z': 0.4687183889123083, 'ar': 5.11508386954684, 'dec': 0.4878393616435365, 'ang_zeta': 0.0028852121230277415, 'ang_theta': 0.002496113304495591, 'ang_z': 0.0028597582311986106}, 'nutation': {'x': 0.3461930457048286, 'y': -0.8127031349845594, 'z': 0.46868325070550965, 'ar': 5.115087075257967, 'dec': 0.4877995836060247, 'dpsi': 1.7724397752215108e-05, 'deps': 4.623967697805032e-05, 'epsm': 0.4090344953255741, 'w': -6.489953776770748}, 'aberration': {'x': 0.34622669314058657, 'y': -0.8126533748739715, 'z': 0.46874467385014457, 'ar': 5.115144196324696, 'dec': 0.48786911792955956, 'lambda_s': 2.9546338179558234, 'epsilon_m': 0.4090294332006951, 'omega_bar': 4.939647965644993}, 'refraction': {'x': 0.3463981365217807, 'y': -0.8129747667747688, 'z': 0.46806020937668613, 'ar': 5.115180129740452, 'dec': 0.4870944119757846, 'R': -159.92869576950548, 'alt': -20.569602217865064}}</t>
+          <t>{'simbad': {'x': 0.7422745682107805, 'y': 0.5587448361350019, 'z': 0.3699090070273623, 'ar': 5.110557462390437, 'dec': 0.4868669741583784, 'ar_deg': 292.81337355406, 'dec_deg': 27.895422803579997, 'pmra': -2.408, 'pmdec': -5.353}, 'proper motion': {'ar': 5.110557161958653, 'dec': 0.48686630629652583, 'pmra': -2.408, 'pmdec': -5.353}, 'precession': {'x': 0.3461891003710981, 'y': -0.8126837013293873, 'z': 0.4687198613007744, 'ar': 5.115091588042937, 'dec': 0.48784102847212446, 'ang_zeta': 0.0028901100151612243, 'ang_theta': 0.002500369232447987, 'ang_z': 0.0028646569776294853}, 'nutation': {'x': 0.3461975984777564, 'y': -0.8127003292529472, 'z': 0.4686847529420872, 'ar': 5.115093061630191, 'dec': 0.4878012841885174, 'dpsi': 1.519641027055965e-05, 'deps': 4.577484563030587e-05, 'epsm': 0.4090343959020549, 'w': -6.5047412493804675}, 'aberration': {'x': 0.34620754707183055, 'y': -0.8126576059514927, 'z': 0.46875147982667165, 'ar': 5.115122378344978, 'dec': 0.4878768228211743, 'lambda_s': 3.229878486430863, 'epsilon_m': 0.40902933380891293, 'omega_bar': 4.939650435148504}, 'refraction': {'x': 0.34662623501995976, 'y': -0.8122849385050677, 'z': 0.4690878722304661, 'ar': 5.115723918735228, 'dec': 0.488257684305156, 'R': 134.83795400374547, 'alt': 24.385124769077716}}</t>
         </is>
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>19h32m18.776s</t>
+          <t>19h32m26.254s</t>
         </is>
       </c>
       <c r="U3" t="inlineStr">
         <is>
-          <t>+27°54'30.435"</t>
+          <t>+27°58'30.377"</t>
         </is>
       </c>
       <c r="V3" t="n">
-        <v>5.115180129740452</v>
+        <v>5.115723918735228</v>
       </c>
       <c r="W3" t="n">
-        <v>0.4870944119757847</v>
+        <v>0.4882576843051559</v>
       </c>
       <c r="X3" t="inlineStr">
         <is>
@@ -808,25 +808,25 @@
       </c>
       <c r="AB3" t="inlineStr">
         <is>
-          <t>19h32m18.776s</t>
+          <t>19h32m26.254s</t>
         </is>
       </c>
       <c r="AC3" t="inlineStr">
         <is>
-          <t>+27°54'30.435"</t>
+          <t>+27°58'30.377"</t>
         </is>
       </c>
       <c r="AD3" t="n">
-        <v>5.115180129740452</v>
+        <v>5.115723918735228</v>
       </c>
       <c r="AE3" t="n">
-        <v>0.4870944119757847</v>
+        <v>0.4882576843051559</v>
       </c>
       <c r="AF3" t="n">
-        <v>-0.001750472409867143</v>
+        <v>293.1093923250301</v>
       </c>
       <c r="AG3" t="n">
-        <v>-0.0005612702044608398</v>
+        <v>27.97510514769373</v>
       </c>
     </row>
     <row r="4">
@@ -881,31 +881,31 @@
         <v>2</v>
       </c>
       <c r="Q4" t="n">
-        <v>292.9305327380487</v>
+        <v>292.9617265017905</v>
       </c>
       <c r="R4" t="n">
-        <v>27.92329730847692</v>
+        <v>27.99009948632038</v>
       </c>
       <c r="S4" t="inlineStr">
         <is>
-          <t>{'simbad': {'x': 0.8212749203440782, 'y': 0.44606842217223996, 'z': 0.3557112142660058, 'ar': 5.107979706849363, 'dec': 0.4871328948917987, 'ar_deg': 292.66567904094, 'dec_deg': 27.910658939290002, 'pmra': 0.174, 'pmdec': -7.135}, 'proper motion': {'ar': 5.107979728521351, 'dec': 0.4871320062157446, 'pmra': 0.174, 'pmdec': -7.135}, 'precession': {'x': 0.3440381908375517, 'y': -0.8134652097759631, 'z': 0.46894783902836457, 'ar': 5.11250433537555, 'dec': 0.48809913018761675, 'ang_zeta': 0.0028852121230277415, 'ang_theta': 0.002496113304495591, 'ang_z': 0.0028597582311986106}, 'nutation': {'x': 0.3440481137336106, 'y': -0.8134812981068563, 'z': 0.46891264971925106, 'ar': 5.1125075874151324, 'dec': 0.4880592888079355, 'dpsi': 1.7724397752215108e-05, 'deps': 4.623967697805032e-05, 'epsm': 0.4090344953255741, 'w': -6.489953776770748}, 'aberration': {'x': 0.3440816903152878, 'y': -0.8134316544168875, 'z': 0.4689741293316512, 'ar': 5.11256449574608, 'dec': 0.48812889665184656, 'lambda_s': 2.9546338179558234, 'epsilon_m': 0.4090294332006951, 'omega_bar': 4.939647965644993}, 'refraction': {'x': 0.344254002452617, 'y': -0.8137533254455236, 'z': 0.46828912769965647, 'ar': 5.11260227589999, 'dec': 0.487353476046193, 'R': -160.0900597454977, 'alt': -20.549295043358285}}</t>
+          <t>{'simbad': {'x': 0.8212749203440782, 'y': 0.44606842217223996, 'z': 0.3557112142660058, 'ar': 5.107979706849363, 'dec': 0.4871328948917987, 'ar_deg': 292.66567904094, 'dec_deg': 27.910658939290002, 'pmra': 0.174, 'pmdec': -7.135}, 'proper motion': {'ar': 5.107979728558305, 'dec': 0.48713200470044465, 'pmra': 0.174, 'pmdec': -7.135}, 'precession': {'x': 0.3440441645241739, 'y': -0.8134618399486644, 'z': 0.4689493019551224, 'ar': 5.112512050840223, 'dec': 0.4881007865333639, 'ang_zeta': 0.0028901100151612243, 'ang_theta': 0.002500369232447987, 'ang_z': 0.0028646569776294853}, 'nutation': {'x': 0.3440526720937682, 'y': -0.8134785082797436, 'z': 0.46891414501175044, 'ar': 5.1125135710768035, 'dec': 0.48806098176282475, 'dpsi': 1.519641027055965e-05, 'deps': 4.577484563030587e-05, 'epsm': 0.4090343959020549, 'w': -6.5047412493804675}, 'aberration': {'x': 0.3440625082083467, 'y': -0.813435862498825, 'z': 0.46898090371162626, 'ar': 5.112542636844218, 'dec': 0.4881365668312743, 'lambda_s': 3.229878486430863, 'epsilon_m': 0.40902933380891293, 'omega_bar': 4.939650435148504}, 'refraction': {'x': 0.3444837538308497, 'y': -0.8130625026553298, 'z': 0.4693189854698593, 'ar': 5.113146709783373, 'dec': 0.48851939399706407, 'R': 135.43679816987049, 'alt': 24.287888626322296}}</t>
         </is>
       </c>
       <c r="T4" t="inlineStr">
         <is>
-          <t>19h31m43.328s</t>
+          <t>19h31m50.814s</t>
         </is>
       </c>
       <c r="U4" t="inlineStr">
         <is>
-          <t>+27°55'23.870"</t>
+          <t>+27°59'24.358"</t>
         </is>
       </c>
       <c r="V4" t="n">
-        <v>5.11260227589999</v>
+        <v>5.113146709783373</v>
       </c>
       <c r="W4" t="n">
-        <v>0.487353476046193</v>
+        <v>0.4885193939970641</v>
       </c>
       <c r="X4" t="inlineStr">
         <is>
@@ -925,25 +925,25 @@
       </c>
       <c r="AB4" t="inlineStr">
         <is>
-          <t>19h31m43.328s</t>
+          <t>19h31m50.814s</t>
         </is>
       </c>
       <c r="AC4" t="inlineStr">
         <is>
-          <t>+27°55'23.870"</t>
+          <t>+27°59'24.358"</t>
         </is>
       </c>
       <c r="AD4" t="n">
-        <v>5.11260227589999</v>
+        <v>5.113146709783373</v>
       </c>
       <c r="AE4" t="n">
-        <v>0.487353476046193</v>
+        <v>0.4885193939970641</v>
       </c>
       <c r="AF4" t="n">
-        <v>-0.001801908597371948</v>
+        <v>292.961742310953</v>
       </c>
       <c r="AG4" t="n">
-        <v>-0.0007845105785797557</v>
+        <v>27.99001588267369</v>
       </c>
     </row>
     <row r="5">
@@ -998,31 +998,31 @@
         <v>4</v>
       </c>
       <c r="Q5" t="n">
-        <v>292.8004933895133</v>
+        <v>292.8316803593627</v>
       </c>
       <c r="R5" t="n">
-        <v>28.00479324090471</v>
+        <v>28.07182854720654</v>
       </c>
       <c r="S5" t="inlineStr">
         <is>
-          <t>{'simbad': {'x': 0.8963735742649112, 'y': 0.34536434220550455, 'z': 0.2779170496614177, 'ar': 5.105714263822092, 'dec': 0.48856493561150405, 'ar_deg': 292.53587871675, 'dec_deg': 27.992708828619996, 'pmra': -3.168, 'pmdec': -17.028}, 'proper motion': {'ar': 5.10571386924245, 'dec': 0.48856281474593305, 'pmra': -3.168, 'pmdec': -17.028}, 'precession': {'x': 0.3419303766555478, 'y': -0.8136273638118496, 'z': 0.4702064763237264, 'ar': 5.1102330977031, 'dec': 0.48952471598089636, 'ang_zeta': 0.0028852121230277415, 'ang_theta': 0.002496113304495591, 'ang_z': 0.0028597582311986106}, 'nutation': {'x': 0.3419402933162705, 'y': -0.81364354461867, 'z': 0.4701712646548588, 'ar': 5.1102363531712545, 'dec': 0.48948481904846736, 'dpsi': 1.7724397752215108e-05, 'deps': 4.623967697805032e-05, 'epsm': 0.4090344953255741, 'w': -6.489953776770748}, 'aberration': {'x': 0.34197376781693306, 'y': -0.813593909880503, 'z': 0.4702328060976249, 'ar': 5.110293109954197, 'dec': 0.48955454974785595, 'lambda_s': 2.9546338179558234, 'epsilon_m': 0.4090294332006951, 'omega_bar': 4.939647965644993}, 'refraction': {'x': 0.3421477422699422, 'y': -0.8139176953431576, 'z': 0.4695454266275668, 'ar': 5.1103326611109, 'dec': 0.48877584839404076, 'R': -160.7800363834425, 'alt': -20.46283702107937}}</t>
+          <t>{'simbad': {'x': 0.8963735742649112, 'y': 0.34536434220550455, 'z': 0.2779170496614177, 'ar': 5.105714263822092, 'dec': 0.48856493561150405, 'ar_deg': 292.53587871675, 'dec_deg': 27.992708828619996, 'pmra': -3.168, 'pmdec': -17.028}, 'proper motion': {'ar': 5.105713868569645, 'dec': 0.4885628111296013, 'pmra': -3.168, 'pmdec': -17.028}, 'precession': {'x': 0.341936346383776, 'y': -0.8136240157885868, 'z': 0.47020792842504044, 'ar': 5.110240803294484, 'dec': 0.4895263613169732, 'ang_zeta': 0.0028901100151612243, 'ang_theta': 0.002500369232447987, 'ang_z': 0.0028646569776294853}, 'nutation': {'x': 0.34194484860769564, 'y': -0.8136407711212419, 'z': 0.4701727513158237, 'ar': 5.110242328938639, 'dec': 0.489486503507348, 'dpsi': 1.519641027055965e-05, 'deps': 4.577484563030587e-05, 'epsm': 0.4090343959020549, 'w': -6.5047412493804675}, 'aberration': {'x': 0.3419545415352607, 'y': -0.8135980888612949, 'z': 0.4702395573797027, 'ar': 5.110271191901631, 'dec': 0.4895621995738007, 'lambda_s': 3.229878486430863, 'epsilon_m': 0.40902933380891293, 'omega_bar': 4.939650435148504}, 'refraction': {'x': 0.3423773186806953, 'y': -0.8132244629389894, 'z': 0.4705780961016037, 'ar': 5.110876976418492, 'dec': 0.48994583520409063, 'R': 135.71931564520767, 'alt': 24.242259468173533}}</t>
         </is>
       </c>
       <c r="T5" t="inlineStr">
         <is>
-          <t>19h31m12.118s</t>
+          <t>19h31m19.603s</t>
         </is>
       </c>
       <c r="U5" t="inlineStr">
         <is>
-          <t>+28°00'17.256"</t>
+          <t>+28°04'18.583"</t>
         </is>
       </c>
       <c r="V5" t="n">
-        <v>5.110332661110899</v>
+        <v>5.110876976418492</v>
       </c>
       <c r="W5" t="n">
-        <v>0.4887758483940408</v>
+        <v>0.4899458352040906</v>
       </c>
       <c r="X5" t="inlineStr">
         <is>
@@ -1042,25 +1042,25 @@
       </c>
       <c r="AB5" t="inlineStr">
         <is>
-          <t>19h31m12.118s</t>
+          <t>19h31m19.603s</t>
         </is>
       </c>
       <c r="AC5" t="inlineStr">
         <is>
-          <t>+28°00'17.256"</t>
+          <t>+28°04'18.583"</t>
         </is>
       </c>
       <c r="AD5" t="n">
-        <v>5.110332661110899</v>
+        <v>5.110876976418492</v>
       </c>
       <c r="AE5" t="n">
-        <v>0.4887758483940408</v>
+        <v>0.4899458352040906</v>
       </c>
       <c r="AF5" t="n">
-        <v>-0.0003554356161430405</v>
+        <v>292.8317255632993</v>
       </c>
       <c r="AG5" t="n">
-        <v>0.002467614476987734</v>
+        <v>28.07163506503066</v>
       </c>
     </row>
     <row r="6">
@@ -1115,31 +1115,31 @@
         <v>5</v>
       </c>
       <c r="Q6" t="n">
-        <v>293.0902968931581</v>
+        <v>293.1214836359269</v>
       </c>
       <c r="R6" t="n">
-        <v>27.84789738782</v>
+        <v>27.91445027759218</v>
       </c>
       <c r="S6" t="inlineStr">
         <is>
-          <t>{'simbad': {'x': 0.7163997389707878, 'y': 0.5530171797645631, 'z': 0.4253744384513908, 'ar': 5.110769316220216, 'dec': 0.48581166950323895, 'ar_deg': 292.82551188438, 'dec_deg': 27.83495830074, 'pmra': -36.737, 'pmdec': -40.447}, 'proper motion': {'ar': 5.110764740566088, 'dec': 0.48580663176247374, 'pmra': -36.737, 'pmdec': -40.447}, 'precession': {'x': 0.34654890904577546, 'y': -0.8130703516474838, 'z': 0.4677824888888209, 'ar': 5.115294672834926, 'dec': 0.48678016680481834, 'ang_zeta': 0.0028852121230277415, 'ang_theta': 0.002496113304495591, 'ang_z': 0.0028597582311986106}, 'nutation': {'x': 0.3465588337352007, 'y': -0.8130863452643168, 'z': 0.4677473355400475, 'ar': 5.1152979074908895, 'dec': 0.486740393955828, 'dpsi': 1.7724397752215108e-05, 'deps': 4.623967697805032e-05, 'epsm': 0.4090344953255741, 'w': -6.489953776770748}, 'aberration': {'x': 0.3465925211897791, 'y': -0.8130366559729136, 'z': 0.4678087432912029, 'ar': 5.11535501450935, 'dec': 0.4868098718433574, 'lambda_s': 2.9546338179558234, 'epsilon_m': 0.4090294332006951, 'omega_bar': 4.939647965644993}, 'refraction': {'x': 0.34676312416177824, 'y': -0.8133564256696246, 'z': 0.4671259578994672, 'ar': 5.115390686433315, 'dec': 0.4860374991749872, 'R': -159.4460245047739, 'alt': -20.63054402871388}}</t>
+          <t>{'simbad': {'x': 0.7163997389707878, 'y': 0.5530171797645631, 'z': 0.4253744384513908, 'ar': 5.110769316220216, 'dec': 0.48581166950323895, 'ar_deg': 292.82551188438, 'dec_deg': 27.83495830074, 'pmra': -36.737, 'pmdec': -40.447}, 'proper motion': {'ar': 5.110764732764045, 'dec': 0.48580662317251766, 'pmra': -36.737, 'pmdec': -40.447}, 'precession': {'x': 0.3465548787657333, 'y': -0.8130669629841538, 'z': 0.4677839562312846, 'ar': 5.115302389556691, 'dec': 0.4867818269889013, 'ang_zeta': 0.0028901100151612243, 'ang_theta': 0.002500369232447987, 'ang_z': 0.0028646569776294853}, 'nutation': {'x': 0.34656338787266755, 'y': -0.8130835429664565, 'z': 0.4677488325408554, 'ar': 5.115303890591102, 'dec': 0.48674208766038873, 'dpsi': 1.519641027055965e-05, 'deps': 4.577484563030587e-05, 'epsm': 0.4090343959020549, 'w': -6.5047412493804675}, 'aberration': {'x': 0.34657338399411886, 'y': -0.813040903273064, 'z': 0.467815539621959, 'ar': 5.115333211674066, 'dec': 0.48681756149715427, 'lambda_s': 3.229878486430863, 'epsilon_m': 0.40902933380891293, 'omega_bar': 4.939650435148504}, 'refraction': {'x': 0.3469924892090688, 'y': -0.812667996061873, 'z': 0.4681526894179646, 'ar': 5.115934997777605, 'dec': 0.4871990662282287, 'R': 135.00168966623244, 'alt': 24.358468398966213}}</t>
         </is>
       </c>
       <c r="T6" t="inlineStr">
         <is>
-          <t>19h32m21.671s</t>
+          <t>19h32m29.156s</t>
         </is>
       </c>
       <c r="U6" t="inlineStr">
         <is>
-          <t>+27°50'52.431"</t>
+          <t>+27°54'52.021"</t>
         </is>
       </c>
       <c r="V6" t="n">
-        <v>5.115390686433315</v>
+        <v>5.115934997777605</v>
       </c>
       <c r="W6" t="n">
-        <v>0.4860374991749872</v>
+        <v>0.4871990662282287</v>
       </c>
       <c r="X6" t="inlineStr">
         <is>
@@ -1159,25 +1159,25 @@
       </c>
       <c r="AB6" t="inlineStr">
         <is>
-          <t>19h32m21.671s</t>
+          <t>19h32m29.156s</t>
         </is>
       </c>
       <c r="AC6" t="inlineStr">
         <is>
-          <t>+27°50'52.431"</t>
+          <t>+27°54'52.021"</t>
         </is>
       </c>
       <c r="AD6" t="n">
-        <v>5.115390686433315</v>
+        <v>5.115934997777605</v>
       </c>
       <c r="AE6" t="n">
-        <v>0.4860374991749872</v>
+        <v>0.4871990662282287</v>
       </c>
       <c r="AF6" t="n">
-        <v>0.002382575213118798</v>
+        <v>293.1214844360286</v>
       </c>
       <c r="AG6" t="n">
-        <v>-0.009132988167369405</v>
+        <v>27.91444913324878</v>
       </c>
     </row>
     <row r="7">
@@ -1232,31 +1232,31 @@
         <v>6</v>
       </c>
       <c r="Q7" t="n">
-        <v>292.8526371735505</v>
+        <v>292.8837800176199</v>
       </c>
       <c r="R7" t="n">
-        <v>28.05378098135077</v>
+        <v>28.12084140040985</v>
       </c>
       <c r="S7" t="inlineStr">
         <is>
-          <t>{'simbad': {'x': 0.888463324428159, 'y': 0.39675014177223034, 'z': 0.23069947149869913, 'ar': 5.106625774103543, 'dec': 0.4894171549136055, 'ar_deg': 292.58810440886, 'dec_deg': 28.041537397849996, 'pmra': 5.823, 'pmdec': 2.919}, 'proper motion': {'ar': 5.106626499367827, 'dec': 0.4894175184798847, 'pmra': 5.823, 'pmdec': 2.919}, 'precession': {'x': 0.3425145474797414, 'y': -0.8129441103478596, 'z': 0.4709624806876609, 'ar': 5.111143665499295, 'dec': 0.4903815190296676, 'ang_zeta': 0.0028852121230277415, 'ang_theta': 0.002496113304495591, 'ang_z': 0.0028597582311986106}, 'nutation': {'x': 0.3425244476997622, 'y': -0.8129603166132129, 'z': 0.4709273047298469, 'ar': 5.111146874711462, 'dec': 0.4903416443437867, 'dpsi': 1.7724397752215108e-05, 'deps': 4.623967697805032e-05, 'epsm': 0.4090344953255741, 'w': -6.489953776770748}, 'aberration': {'x': 0.3425579163436494, 'y': -0.8129105673215905, 'z': 0.47098883584134726, 'ar': 5.11120373556162, 'dec': 0.49041139520382043, 'lambda_s': 2.9546338179558234, 'epsilon_m': 0.4090294332006951, 'omega_bar': 4.939647965644993}, 'refraction': {'x': 0.34273229398390753, 'y': -0.8132357307293872, 'z': 0.4703001391936512, 'ar': 5.111242741826796, 'dec': 0.4896308457579368, 'R': -161.1563057420432, 'alt': -20.415941717928774}}</t>
+          <t>{'simbad': {'x': 0.888463324428159, 'y': 0.39675014177223034, 'z': 0.23069947149869913, 'ar': 5.106625774103543, 'dec': 0.4894171549136055, 'ar_deg': 292.58810440886, 'dec_deg': 28.041537397849996, 'pmra': 5.823, 'pmdec': 2.919}, 'proper motion': {'ar': 5.10662650060449, 'dec': 0.4894175190998091, 'pmra': 5.823, 'pmdec': 2.919}, 'precession': {'x': 0.3425205080671998, 'y': -0.8129407541134435, 'z': 0.47096393901747174, 'ar': 5.111151369473162, 'dec': 0.49038317217833344, 'ang_zeta': 0.0028901100151612243, 'ang_theta': 0.002500369232447987, 'ang_z': 0.0028646569776294853}, 'nutation': {'x': 0.34252899619517435, 'y': -0.8129575359085003, 'z': 0.4709287967146469, 'ar': 5.111152850097802, 'dec': 0.49034333560743953, 'dpsi': 1.519641027055965e-05, 'deps': 4.577484563030587e-05, 'epsm': 0.4090343959020549, 'w': -6.5047412493804675}, 'aberration': {'x': 0.3425386941632343, 'y': -0.8129147441344517, 'z': 0.4709956069537849, 'ar': 5.111181816450887, 'dec': 0.49041907100661614, 'lambda_s': 3.229878486430863, 'epsilon_m': 0.40902933380891293, 'omega_bar': 4.939650435148504}, 'refraction': {'x': 0.3429599885294634, 'y': -0.8125416352155431, 'z': 0.47133272463210185, 'ar': 5.111786286994242, 'dec': 0.4908012708682849, 'R': 135.31152915643793, 'alt': 24.308170653833677}}</t>
         </is>
       </c>
       <c r="T7" t="inlineStr">
         <is>
-          <t>19h31m24.633s</t>
+          <t>19h31m32.107s</t>
         </is>
       </c>
       <c r="U7" t="inlineStr">
         <is>
-          <t>+28°03'13.612"</t>
+          <t>+28°07'15.029"</t>
         </is>
       </c>
       <c r="V7" t="n">
-        <v>5.111242741826796</v>
+        <v>5.111786286994242</v>
       </c>
       <c r="W7" t="n">
-        <v>0.4896308457579368</v>
+        <v>0.4908012708682849</v>
       </c>
       <c r="X7" t="inlineStr">
         <is>
@@ -1276,25 +1276,25 @@
       </c>
       <c r="AB7" t="inlineStr">
         <is>
-          <t>19h31m24.633s</t>
+          <t>19h31m32.107s</t>
         </is>
       </c>
       <c r="AC7" t="inlineStr">
         <is>
-          <t>+28°03'13.612"</t>
+          <t>+28°07'15.029"</t>
         </is>
       </c>
       <c r="AD7" t="n">
-        <v>5.111242741826796</v>
+        <v>5.111786286994242</v>
       </c>
       <c r="AE7" t="n">
-        <v>0.4896308457579368</v>
+        <v>0.4908012708682849</v>
       </c>
       <c r="AF7" t="n">
-        <v>-0.0002643299757210116</v>
+        <v>292.883830322974</v>
       </c>
       <c r="AG7" t="n">
-        <v>-0.0006714295478182919</v>
+        <v>28.12068072795756</v>
       </c>
     </row>
     <row r="8">
@@ -1349,31 +1349,31 @@
         <v>7</v>
       </c>
       <c r="Q8" t="n">
-        <v>292.8535391596128</v>
+        <v>292.8848197105605</v>
       </c>
       <c r="R8" t="n">
-        <v>27.81511943174781</v>
+        <v>27.88183632469486</v>
       </c>
       <c r="S8" t="inlineStr">
         <is>
-          <t>{'simbad': {'x': 0.81317961965919, 'y': 0.3633906955498259, 'z': 0.4546274392937025, 'ar': 5.1066304095434, 'dec': 0.485243070890621, 'ar_deg': 292.58836999999994, 'dec_deg': 27.80238, 'pmra': nan, 'pmdec': nan}, 'proper motion': {'ar': 5.1066304095434, 'dec': 0.485243070890621, 'pmra': 0, 'pmdec': 0}, 'precession': {'x': 0.3432881261679789, 'y': -0.8147432050550635, 'z': 0.4672759059149965, 'ar': 5.111159898059906, 'dec': 0.486207094625581, 'ang_zeta': 0.0028852121230277415, 'ang_theta': 0.002496113304495591, 'ang_z': 0.0028597582311986106}, 'nutation': {'x': 0.3432980816333522, 'y': -0.8147592282721567, 'z': 0.46724065222561706, 'ar': 5.11116323779227, 'dec': 0.48616722033819154, 'dpsi': 1.7724397752215108e-05, 'deps': 4.623967697805032e-05, 'epsm': 0.4090344953255741, 'w': -6.489953776770748}, 'aberration': {'x': 0.3433316874227683, 'y': -0.8147098026054076, 'z': 0.4673021398946215, 'ar': 5.11121997410837, 'dec': 0.48623676756156803, 'lambda_s': 2.9546338179558234, 'epsilon_m': 0.4090294332006951, 'omega_bar': 4.939647965644993}, 'refraction': {'x': 0.34350295185300517, 'y': -0.8150284966248305, 'z': 0.4666200507455082, 'ar': 5.111258484453391, 'dec': 0.4854654159194534, 'R': -159.2576726823434, 'alt': -20.65440653135829}}</t>
+          <t>{'simbad': {'x': 0.81317961965919, 'y': 0.3633906955498259, 'z': 0.4546274392937025, 'ar': 5.1066304095434, 'dec': 0.485243070890621, 'ar_deg': 292.58836999999994, 'dec_deg': 27.80238, 'pmra': nan, 'pmdec': nan}, 'proper motion': {'ar': 5.1066304095434, 'dec': 0.485243070890621, 'pmra': 0, 'pmdec': 0}, 'precession': {'x': 0.34329411917983726, 'y': -0.8147398419356896, 'z': 0.4672773669879028, 'ar': 5.111167621804524, 'dec': 0.4862087472151768, 'ang_zeta': 0.0028901100151612243, 'ang_theta': 0.002500369232447987, 'ang_z': 0.0028646569776294853}, 'nutation': {'x': 0.34330265467355314, 'y': -0.8147564441901851, 'z': 0.4672421470122926, 'ar': 5.111169227025609, 'dec': 0.48616891102512816, 'dpsi': 1.519641027055965e-05, 'deps': 4.577484563030587e-05, 'epsm': 0.4090343959020549, 'w': -6.5047412493804675}, 'aberration': {'x': 0.34331250624335774, 'y': -0.8147140147414706, 'z': 0.4673088884675095, 'ar': 5.111198130842711, 'dec': 0.4862444008657211, 'lambda_s': 3.229878486430863, 'epsilon_m': 0.40902933380891293, 'omega_bar': 4.939650435148504}, 'refraction': {'x': 0.34373633480627475, 'y': -0.8143397093829498, 'z': 0.4676496229615092, 'ar': 5.111804433059267, 'dec': 0.48662984536807996, 'R': 136.17151408274637, 'alt': 24.169548476974306}}</t>
         </is>
       </c>
       <c r="T8" t="inlineStr">
         <is>
-          <t>19h31m24.849s</t>
+          <t>19h31m32.357s</t>
         </is>
       </c>
       <c r="U8" t="inlineStr">
         <is>
-          <t>+27°48'54.430"</t>
+          <t>+27°52'54.611"</t>
         </is>
       </c>
       <c r="V8" t="n">
-        <v>5.11125848445339</v>
+        <v>5.111804433059266</v>
       </c>
       <c r="W8" t="n">
-        <v>0.4854654159194535</v>
+        <v>0.48662984536808</v>
       </c>
       <c r="X8" t="inlineStr">
         <is>
@@ -1393,25 +1393,25 @@
       </c>
       <c r="AB8" t="inlineStr">
         <is>
-          <t>19h31m24.849s</t>
+          <t>19h31m32.357s</t>
         </is>
       </c>
       <c r="AC8" t="inlineStr">
         <is>
-          <t>+27°48'54.430"</t>
+          <t>+27°52'54.611"</t>
         </is>
       </c>
       <c r="AD8" t="n">
-        <v>5.11125848445339</v>
+        <v>5.111804433059266</v>
       </c>
       <c r="AE8" t="n">
-        <v>0.4854654159194535</v>
+        <v>0.48662984536808</v>
       </c>
       <c r="AF8" t="n">
-        <v>0.0009558290826134908</v>
+        <v>292.8848188495289</v>
       </c>
       <c r="AG8" t="n">
-        <v>-0.002694766099967438</v>
+        <v>27.88174417494995</v>
       </c>
     </row>
     <row r="9">
@@ -1466,31 +1466,31 @@
         <v>8</v>
       </c>
       <c r="Q9" t="n">
-        <v>292.9538373948023</v>
+        <v>292.9849928248141</v>
       </c>
       <c r="R9" t="n">
-        <v>27.97789020831811</v>
+        <v>28.04475056033824</v>
       </c>
       <c r="S9" t="inlineStr">
         <is>
-          <t>{'simbad': {'x': 0.8262121933548849, 'y': 0.4741925761710259, 'z': 0.304162476738989, 'ar': 5.108389365583733, 'dec': 0.4880861207025677, 'ar_deg': 292.68915075746, 'dec_deg': 27.96527475517, 'pmra': -1.078, 'pmdec': -1.54}, 'proper motion': {'ar': 5.10838923131705, 'dec': 0.4880859288930199, 'pmra': -1.078, 'pmdec': -1.54}, 'precession': {'x': 0.34419441301499076, 'y': -0.8129124414908462, 'z': 0.46979098386267215, 'ar': 5.1129112328226825, 'dec': 0.48905399211190576, 'ang_zeta': 0.0028852121230277415, 'ang_theta': 0.002496113304495591, 'ang_z': 0.0028597582311986106}, 'nutation': {'x': 0.3442043209781056, 'y': -0.8129285662687268, 'z': 0.46975582121382353, 'ar': 5.112914446227553, 'dec': 0.48901416070587694, 'dpsi': 1.7724397752215108e-05, 'deps': 4.623967697805032e-05, 'epsm': 0.4090344953255741, 'w': -6.489953776770748}, 'aberration': {'x': 0.34423787604816103, 'y': -0.8128788269611255, 'z': 0.46981730212089423, 'ar': 5.11297141828746, 'dec': 0.4890838053566425, 'lambda_s': 2.9546338179558234, 'epsilon_m': 0.4090294332006951, 'omega_bar': 4.939647965644993}, 'refraction': {'x': 0.34441079356717585, 'y': -0.8132019982194064, 'z': 0.4691308083747987, 'ar': 5.113009018891388, 'dec': 0.4883063018966332, 'R': -160.5177351551529, 'alt': -20.49563376796375}}</t>
+          <t>{'simbad': {'x': 0.8262121933548849, 'y': 0.4741925761710259, 'z': 0.304162476738989, 'ar': 5.108389365583733, 'dec': 0.4880861207025677, 'ar_deg': 292.68915075746, 'dec_deg': 27.96527475517, 'pmra': -1.078, 'pmdec': -1.54}, 'proper motion': {'ar': 5.1083892310881085, 'dec': 0.48808592856596145, 'pmra': -1.078, 'pmdec': -1.54}, 'precession': {'x': 0.34420037726204944, 'y': -0.8129090697131501, 'z': 0.46979244850334023, 'ar': 5.11291894357657, 'dec': 0.48905565124007433, 'ang_zeta': 0.0028901100151612243, 'ang_theta': 0.002500369232447987, 'ang_z': 0.0028646569776294853}, 'nutation': {'x': 0.34420887202851524, 'y': -0.8129257744618033, 'z': 0.4697573178062632, 'ar': 5.112920426541764, 'dec': 0.48901585599272845, 'dpsi': 1.519641027055965e-05, 'deps': 4.577484563030587e-05, 'epsm': 0.4090343959020549, 'w': -6.5047412493804675}, 'aberration': {'x': 0.344218689287025, 'y': -0.8128830300058366, 'z': 0.46982408779675466, 'ar': 5.112949547316475, 'dec': 0.48909149222680626, 'lambda_s': 3.229878486430863, 'epsilon_m': 0.40902933380891293, 'omega_bar': 4.939650435148504}, 'refraction': {'x': 0.34463892697417314, 'y': -0.8125100648928588, 'z': 0.47016104098690775, 'ar': 5.113552783724967, 'dec': 0.489473235178427, 'R': 135.13732117198572, 'alt': 24.336427448933634}}</t>
         </is>
       </c>
       <c r="T9" t="inlineStr">
         <is>
-          <t>19h31m48.921s</t>
+          <t>19h31m56.398s</t>
         </is>
       </c>
       <c r="U9" t="inlineStr">
         <is>
-          <t>+27°58'40.405"</t>
+          <t>+28°02'41.102"</t>
         </is>
       </c>
       <c r="V9" t="n">
-        <v>5.113009018891388</v>
+        <v>5.113552783724967</v>
       </c>
       <c r="W9" t="n">
-        <v>0.4883063018966333</v>
+        <v>0.4894732351784269</v>
       </c>
       <c r="X9" t="inlineStr">
         <is>
@@ -1510,25 +1510,25 @@
       </c>
       <c r="AB9" t="inlineStr">
         <is>
-          <t>19h31m48.921s</t>
+          <t>19h31m56.398s</t>
         </is>
       </c>
       <c r="AC9" t="inlineStr">
         <is>
-          <t>+27°58'40.405"</t>
+          <t>+28°02'41.102"</t>
         </is>
       </c>
       <c r="AD9" t="n">
-        <v>5.113009018891388</v>
+        <v>5.113552783724967</v>
       </c>
       <c r="AE9" t="n">
-        <v>0.4883063018966333</v>
+        <v>0.4894732351784269</v>
       </c>
       <c r="AF9" t="n">
-        <v>-0.001596827788034716</v>
+        <v>292.9850144897874</v>
       </c>
       <c r="AG9" t="n">
-        <v>-0.001474861039760356</v>
+        <v>28.04467703484197</v>
       </c>
     </row>
     <row r="10">
@@ -1583,31 +1583,31 @@
         <v>9</v>
       </c>
       <c r="Q10" t="n">
-        <v>292.9235354446233</v>
+        <v>292.9547226216448</v>
       </c>
       <c r="R10" t="n">
-        <v>27.93853720568747</v>
+        <v>28.00536757839082</v>
       </c>
       <c r="S10" t="inlineStr">
         <is>
-          <t>{'simbad': {'x': 0.8290374353702145, 'y': 0.4428595014714414, 'z': 0.34142699470200644, 'ar': 5.107858546571783, 'dec': 0.48739888718441626, 'ar_deg': 292.65873706839, 'dec_deg': 27.92589917504, 'pmra': -1.631, 'pmdec': -0.266}, 'proper motion': {'ar': 5.107858343428034, 'dec': 0.4873988540536762, 'pmra': -1.631, 'pmdec': -0.266}, 'precession': {'x': 0.34389006395544547, 'y': -0.8133920892488692, 'z': 0.4691832617006701, 'ar': 5.11238210131995, 'dec': 0.4883656977173774, 'ang_zeta': 0.0028852121230277415, 'ang_theta': 0.002496113304495591, 'ang_z': 0.0028597582311986106}, 'nutation': {'x': 0.34389998400283345, 'y': -0.813408190874557, 'z': 0.46914807472804554, 'ar': 5.11238534757242, 'dec': 0.48832585334263534, 'dpsi': 1.7724397752215108e-05, 'deps': 4.623967697805032e-05, 'epsm': 0.4090344953255741, 'w': -6.489953776770748}, 'aberration': {'x': 0.3439335488621983, 'y': -0.8133585329472639, 'z': 0.46920955963079974, 'ar': 5.1124422534947165, 'dec': 0.48839547703297714, 'lambda_s': 2.9546338179558234, 'epsilon_m': 0.4090294332006951, 'omega_bar': 4.939647965644993}, 'refraction': {'x': 0.34410609159247413, 'y': -0.8136806113070127, 'z': 0.46852413012778493, 'ar': 5.112480150090989, 'dec': 0.4876194624301825, 'R': -160.2133382310432, 'alt': -20.533803193021196}}</t>
+          <t>{'simbad': {'x': 0.8290374353702145, 'y': 0.4428595014714414, 'z': 0.34142699470200644, 'ar': 5.107858546571783, 'dec': 0.48739888718441626, 'ar_deg': 292.65873706839, 'dec_deg': 27.92589917504, 'pmra': -1.631, 'pmdec': -0.266}, 'proper motion': {'ar': 5.1078583430816495, 'dec': 0.48739885399718436, 'pmra': -1.631, 'pmdec': -0.266}, 'precession': {'x': 0.3438960353420087, 'y': -0.8133887203764192, 'z': 0.4691847252846783, 'ar': 5.112389814949498, 'dec': 0.48836735504189954, 'ang_zeta': 0.0028901100151612243, 'ang_theta': 0.002500369232447987, 'ang_z': 0.0028646569776294853}, 'nutation': {'x': 0.3439045404692378, 'y': -0.8134054015493513, 'z': 0.46914957079270647, 'ar': 5.112391329774862, 'dec': 0.4883275474115615, 'dpsi': 1.519641027055965e-05, 'deps': 4.577484563030587e-05, 'epsm': 0.4090343959020549, 'w': -6.5047412493804675}, 'aberration': {'x': 0.34391436190205027, 'y': -0.8133627373353001, 'z': 0.4692163351716697, 'ar': 5.112420387566921, 'dec': 0.488403149613156, 'lambda_s': 3.229878486430863, 'epsilon_m': 0.40902933380891293, 'omega_bar': 4.939650435148504}, 'refraction': {'x': 0.344335574466878, 'y': -0.8129894176166732, 'z': 0.469554276947689, 'ar': 5.113024469014416, 'dec': 0.4887858724741911, 'R': 135.41285261286495, 'alt': 24.29176322237684}}</t>
         </is>
       </c>
       <c r="T10" t="inlineStr">
         <is>
-          <t>19h31m41.649s</t>
+          <t>19h31m49.133s</t>
         </is>
       </c>
       <c r="U10" t="inlineStr">
         <is>
-          <t>+27°56'18.734"</t>
+          <t>+28°00'19.323"</t>
         </is>
       </c>
       <c r="V10" t="n">
-        <v>5.112480150090989</v>
+        <v>5.113024469014416</v>
       </c>
       <c r="W10" t="n">
-        <v>0.4876194624301825</v>
+        <v>0.488785872474191</v>
       </c>
       <c r="X10" t="inlineStr">
         <is>
@@ -1627,25 +1627,25 @@
       </c>
       <c r="AB10" t="inlineStr">
         <is>
-          <t>19h31m41.649s</t>
+          <t>19h31m49.133s</t>
         </is>
       </c>
       <c r="AC10" t="inlineStr">
         <is>
-          <t>+27°56'18.734"</t>
+          <t>+28°00'19.323"</t>
         </is>
       </c>
       <c r="AD10" t="n">
-        <v>5.112480150090989</v>
+        <v>5.113024469014416</v>
       </c>
       <c r="AE10" t="n">
-        <v>0.4876194624301825</v>
+        <v>0.488785872474191</v>
       </c>
       <c r="AF10" t="n">
-        <v>-0.001756317578383459</v>
+        <v>292.9547413830394</v>
       </c>
       <c r="AG10" t="n">
-        <v>-0.000763949348034032</v>
+        <v>28.00527735697851</v>
       </c>
     </row>
     <row r="11">
@@ -1679,7 +1679,7 @@
         <v>-2.81</v>
       </c>
       <c r="J11" t="n">
-        <v>5.948888893626201e-05</v>
+        <v>5.948888893626203e-05</v>
       </c>
       <c r="K11" t="n">
         <v>1257.659057617188</v>
@@ -1700,31 +1700,31 @@
         <v>10</v>
       </c>
       <c r="Q11" t="n">
-        <v>293.0036246186693</v>
+        <v>293.0346980368223</v>
       </c>
       <c r="R11" t="n">
-        <v>28.09670465704639</v>
+        <v>28.16369487082316</v>
       </c>
       <c r="S11" t="inlineStr">
         <is>
-          <t>{'simbad': {'x': 0.8261113084204398, 'y': 0.5308830988331615, 'z': 0.1889530139298358, 'ar': 5.109264509843677, 'dec': 0.49016242167152185, 'ar_deg': 292.73929283001996, 'dec_deg': 28.08423803769, 'pmra': -2.519, 'pmdec': -2.657}, 'proper motion': {'ar': 5.10926419609806, 'dec': 0.4901620907377761, 'pmra': -2.519, 'pmdec': -2.657}, 'precession': {'x': 0.344518745162723, 'y': -0.8117124727564865, 'z': 0.4716245284154047, 'ar': 5.113780512970874, 'dec': 0.4911321601239684, 'ang_zeta': 0.0028852121230277415, 'ang_theta': 0.002496113304495591, 'ang_z': 0.0028597582311986106}, 'nutation': {'x': 0.3445286206862102, 'y': -0.8117286770441637, 'z': 0.4715894235372431, 'ar': 5.113783642402272, 'dec': 0.49109235004734136, 'dpsi': 1.7724397752215108e-05, 'deps': 4.623967697805032e-05, 'epsm': 0.4090344953255741, 'w': -6.489953776770748}, 'aberration': {'x': 0.34456212829426647, 'y': -0.8116787305896236, 'z': 0.4716509069786072, 'ar': 5.1138407521379206, 'dec': 0.491162074832639, 'lambda_s': 2.9546338179558234, 'epsilon_m': 0.4090294332006951, 'omega_bar': 4.939647965644993}, 'refraction': {'x': 0.3447363795669349, 'y': -0.812005189786025, 'z': 0.4709611452802057, 'ar': 5.113877969873293, 'dec': 0.4903800052258837, 'R': -161.4554612333064, 'alt': -20.378783977494592}}</t>
+          <t>{'simbad': {'x': 0.8261113084204398, 'y': 0.5308830988331615, 'z': 0.1889530139298358, 'ar': 5.109264509843677, 'dec': 0.49016242167152185, 'ar_deg': 292.73929283001996, 'dec_deg': 28.08423803769, 'pmra': -2.519, 'pmdec': -2.657}, 'proper motion': {'ar': 5.109264195563085, 'dec': 0.49016209017349416, 'pmra': -2.519, 'pmdec': -2.657}, 'precession': {'x': 0.34452468964716254, 'y': -0.8117090980105425, 'z': 0.47162599422682155, 'ar': 5.113788213728855, 'dec': 0.49113382242035136, 'ang_zeta': 0.0028901100151612243, 'ang_theta': 0.002500369232447987, 'ang_z': 0.0028646569776294853}, 'nutation': {'x': 0.344533156600745, 'y': -0.8117258821691902, 'z': 0.47159092041660056, 'ar': 5.113789615692058, 'dec': 0.4910940475400469, 'dpsi': 1.519641027055965e-05, 'deps': 4.577484563030587e-05, 'epsm': 0.4090343959020549, 'w': -6.5047412493804675}, 'aberration': {'x': 0.34454293187620477, 'y': -0.8116829235890636, 'z': 0.4716577145007376, 'ar': 5.113818854840497, 'dec': 0.49116979500638097, 'lambda_s': 3.229878486430863, 'epsilon_m': 0.40902933380891293, 'omega_bar': 4.939650435148504}, 'refraction': {'x': 0.3449610084363729, 'y': -0.8113108100655345, 'z': 0.4719922373613434, 'ar': 5.114420303329913, 'dec': 0.4915492050229031, 'R': 134.49383465654233, 'alt': 24.44132074560874}}</t>
         </is>
       </c>
       <c r="T11" t="inlineStr">
         <is>
-          <t>19h32m0.870s</t>
+          <t>19h32m8.328s</t>
         </is>
       </c>
       <c r="U11" t="inlineStr">
         <is>
-          <t>+28°05'48.137"</t>
+          <t>+28°09'49.302"</t>
         </is>
       </c>
       <c r="V11" t="n">
-        <v>5.113877969873293</v>
+        <v>5.114420303329913</v>
       </c>
       <c r="W11" t="n">
-        <v>0.4903800052258837</v>
+        <v>0.4915492050229032</v>
       </c>
       <c r="X11" t="inlineStr">
         <is>
@@ -1744,25 +1744,25 @@
       </c>
       <c r="AB11" t="inlineStr">
         <is>
-          <t>19h32m0.870s</t>
+          <t>19h32m8.328s</t>
         </is>
       </c>
       <c r="AC11" t="inlineStr">
         <is>
-          <t>+28°05'48.137"</t>
+          <t>+28°09'49.302"</t>
         </is>
       </c>
       <c r="AD11" t="n">
-        <v>5.113877969873293</v>
+        <v>5.114420303329913</v>
       </c>
       <c r="AE11" t="n">
-        <v>0.4903800052258837</v>
+        <v>0.4915492050229032</v>
       </c>
       <c r="AF11" t="n">
-        <v>-0.0006061503339651608</v>
+        <v>293.0347259946798</v>
       </c>
       <c r="AG11" t="n">
-        <v>7.64065512015577e-06</v>
+        <v>28.16367494296426</v>
       </c>
     </row>
     <row r="12">
@@ -1817,31 +1817,31 @@
         <v>12</v>
       </c>
       <c r="Q12" t="n">
-        <v>292.9409173355272</v>
+        <v>292.9720688609363</v>
       </c>
       <c r="R12" t="n">
-        <v>27.99163315128364</v>
+        <v>28.05852480795233</v>
       </c>
       <c r="S12" t="inlineStr">
         <is>
-          <t>{'simbad': {'x': 0.8358430514289432, 'y': 0.46551566672851213, 'z': 0.2909665915672484, 'ar': 5.108164618902049, 'dec': 0.48832736255872994, 'ar_deg': 292.67627372114, 'dec_deg': 27.979096895370002, 'pmra': -1.855, 'pmdec': -4.197}, 'proper motion': {'ar': 5.1081643878587295, 'dec': 0.4883268398154364, 'pmra': -1.855, 'pmdec': -4.197}, 'precession': {'x': 0.3439669351386683, 'y': -0.812886065196635, 'z': 0.4700031835428815, 'ar': 5.112685563205163, 'dec': 0.48929438475147957, 'ang_zeta': 0.0028852121230277415, 'ang_theta': 0.002496113304495591, 'ang_z': 0.0028597582311986106}, 'nutation': {'x': 0.34397684117699856, 'y': -0.8129022034858271, 'z': 0.4699680205096741, 'ar': 5.11268877383178, 'dec': 0.4892545478128465, 'dpsi': 1.7724397752215108e-05, 'deps': 4.623967697805032e-05, 'epsm': 0.4090344953255741, 'w': -6.489953776770748}, 'aberration': {'x': 0.34401038288699454, 'y': -0.8128524574299992, 'z': 0.4700295085587235, 'ar': 5.112745733856254, 'dec': 0.4893242094678124, 'lambda_s': 2.9546338179558234, 'epsilon_m': 0.4090294332006951, 'omega_bar': 4.939647965644993}, 'refraction': {'x': 0.3441835394395924, 'y': -0.8131759923681032, 'z': 0.46934262177537756, 'ar': 5.112783521317484, 'dec': 0.4885461615002955, 'R': -160.63136242517, 'alt': -20.481415744369478}}</t>
+          <t>{'simbad': {'x': 0.8358430514289432, 'y': 0.46551566672851213, 'z': 0.2909665915672484, 'ar': 5.108164618902049, 'dec': 0.48832736255872994, 'ar_deg': 292.67627372114, 'dec_deg': 27.979096895370002, 'pmra': -1.855, 'pmdec': -4.197}, 'proper motion': {'ar': 5.1081643874647735, 'dec': 0.48832683892409606, 'pmra': -1.855, 'pmdec': -4.197}, 'precession': {'x': 0.34397289819480603, 'y': -0.8128826959481007, 'z': 0.4700046467170438, 'ar': 5.1126932723871725, 'dec': 0.4892960424305228, 'ang_zeta': 0.0028901100151612243, 'ang_theta': 0.002500369232447987, 'ang_z': 0.0028646569776294853}, 'nutation': {'x': 0.34398139131105465, 'y': -0.8128994135817627, 'z': 0.46996951585197255, 'ar': 5.112694752911308, 'dec': 0.48925624190033123, 'dpsi': 1.519641027055965e-05, 'deps': 4.577484563030587e-05, 'epsm': 0.4090343959020549, 'w': -6.5047412493804675}, 'aberration': {'x': 0.3439911907273183, 'y': -0.8128566569580036, 'z': 0.4700362921531274, 'ar': 5.112723855083249, 'dec': 0.4893318949636412, 'lambda_s': 3.229878486430863, 'epsilon_m': 0.40902933380891293, 'omega_bar': 4.939650435148504}, 'refraction': {'x': 0.3444115204081009, 'y': -0.8124836937284015, 'z': 0.47037320505704133, 'ar': 5.113327218002891, 'dec': 0.4897136411512778, 'R': 135.1449987646842, 'alt': 24.33518087590709}}</t>
         </is>
       </c>
       <c r="T12" t="inlineStr">
         <is>
-          <t>19h31m45.820s</t>
+          <t>19h31m53.297s</t>
         </is>
       </c>
       <c r="U12" t="inlineStr">
         <is>
-          <t>+27°59'29.879"</t>
+          <t>+28°03'30.689"</t>
         </is>
       </c>
       <c r="V12" t="n">
-        <v>5.112783521317483</v>
+        <v>5.113327218002891</v>
       </c>
       <c r="W12" t="n">
-        <v>0.4885461615002955</v>
+        <v>0.4897136411512778</v>
       </c>
       <c r="X12" t="inlineStr">
         <is>
@@ -1861,25 +1861,25 @@
       </c>
       <c r="AB12" t="inlineStr">
         <is>
-          <t>19h31m45.820s</t>
+          <t>19h31m53.297s</t>
         </is>
       </c>
       <c r="AC12" t="inlineStr">
         <is>
-          <t>+27°59'29.879"</t>
+          <t>+28°03'30.689"</t>
         </is>
       </c>
       <c r="AD12" t="n">
-        <v>5.112783521317483</v>
+        <v>5.113327218002891</v>
       </c>
       <c r="AE12" t="n">
-        <v>0.4885461615002955</v>
+        <v>0.4897136411512778</v>
       </c>
       <c r="AF12" t="n">
-        <v>0.001305257800936488</v>
+        <v>292.9720941337063</v>
       </c>
       <c r="AG12" t="n">
-        <v>0.001169315358261258</v>
+        <v>28.05843950789126</v>
       </c>
     </row>
     <row r="13">
@@ -1913,7 +1913,7 @@
         <v>0</v>
       </c>
       <c r="J13" t="n">
-        <v>0.0005523598064026557</v>
+        <v>0.0005523598064026558</v>
       </c>
       <c r="K13" t="n">
         <v>1378.947143554688</v>
@@ -1934,31 +1934,31 @@
         <v>14</v>
       </c>
       <c r="Q13" t="n">
-        <v>292.8623173063237</v>
+        <v>292.8934195880882</v>
       </c>
       <c r="R13" t="n">
-        <v>28.12065380659048</v>
+        <v>28.18780442058016</v>
       </c>
       <c r="S13" t="inlineStr">
         <is>
-          <t>{'simbad': {'x': 0.8966671083272044, 'y': 0.4106590254296342, 'z': 0.1653700749147576, 'ar': 5.106791332135402, 'dec': 0.49058064800361184, 'ar_deg': 292.59759018535, 'dec_deg': 28.108200641399996, 'pmra': 59.919, 'pmdec': 49.543}, 'proper motion': {'ar': 5.106798795145982, 'dec': 0.4905868186662255, 'pmra': 59.919, 'pmdec': 49.543}, 'precession': {'x': 0.34243765624013806, 'y': -0.8123780580448775, 'z': 0.4719940067373683, 'ar': 5.111312588661198, 'dec': 0.4915512120232982, 'ang_zeta': 0.0028852121230277415, 'ang_theta': 0.002496113304495591, 'ang_z': 0.0028597582311986106}, 'nutation': {'x': 0.34244753998324684, 'y': -0.812394313258799, 'z': 0.47195885641037316, 'ar': 5.1113157574948005, 'dec': 0.4915113414677125, 'dpsi': 1.7724397752215108e-05, 'deps': 4.623967697805032e-05, 'epsm': 0.4090344953255741, 'w': -6.489953776770748}, 'aberration': {'x': 0.3424809743766186, 'y': -0.8123444641145623, 'z': 0.4720203955471274, 'ar': 5.111372668405846, 'dec': 0.4915811450639365, 'lambda_s': 2.9546338179558234, 'epsilon_m': 0.4090294332006951, 'omega_bar': 4.939647965644993}, 'refraction': {'x': 0.34265619001879744, 'y': -0.8126714712613468, 'z': 0.4713298369928637, 'ar': 5.11141169201572, 'dec': 0.4907979967384806, 'R': -161.69178857743105, 'alt': -20.349509000929707}}</t>
+          <t>{'simbad': {'x': 0.8966671083272044, 'y': 0.4106590254296342, 'z': 0.1653700749147576, 'ar': 5.106791332135402, 'dec': 0.49058064800361184, 'ar_deg': 292.59759018535, 'dec_deg': 28.108200641399996, 'pmra': 59.919, 'pmdec': 49.543}, 'proper motion': {'ar': 5.106798807871316, 'dec': 0.49058682918795, 'pmra': 59.919, 'pmdec': 49.543}, 'precession': {'x': 0.34244361438488213, 'y': -0.8123746943189383, 'z': 0.4719954734923095, 'ar': 5.111320298350915, 'dec': 0.4915528757627171, 'ang_zeta': 0.0028901100151612243, 'ang_theta': 0.002500369232447987, 'ang_z': 0.0028646569776294853}, 'nutation': {'x': 0.34245208838585056, 'y': -0.812391524405109, 'z': 0.4719603566348688, 'ar': 5.111321740264549, 'dec': 0.4915130431353255, 'dpsi': 1.519641027055965e-05, 'deps': 4.577484563030587e-05, 'epsm': 0.4090343959020549, 'w': -6.5047412493804675}, 'aberration': {'x': 0.342461750185466, 'y': -0.8123486243576092, 'z': 0.47202718371319125, 'ar': 5.111350741474608, 'dec': 0.491588845013255, 'lambda_s': 3.229878486430863, 'epsilon_m': 0.40902933380891293, 'omega_bar': 4.939650435148504}, 'refraction': {'x': 0.3428821593057271, 'y': -0.8119759012257528, 'z': 0.47236316606872303, 'ar': 5.111954529237394, 'dec': 0.4919699960473362, 'R': 135.0287186190367, 'alt': 24.35407313797423}}</t>
         </is>
       </c>
       <c r="T13" t="inlineStr">
         <is>
-          <t>19h31m26.956s</t>
+          <t>19h31m34.421s</t>
         </is>
       </c>
       <c r="U13" t="inlineStr">
         <is>
-          <t>+28°07'14.354"</t>
+          <t>+28°11'16.096"</t>
         </is>
       </c>
       <c r="V13" t="n">
-        <v>5.11141169201572</v>
+        <v>5.111954529237394</v>
       </c>
       <c r="W13" t="n">
-        <v>0.4907979967384806</v>
+        <v>0.4919699960473362</v>
       </c>
       <c r="X13" t="inlineStr">
         <is>
@@ -1978,25 +1978,25 @@
       </c>
       <c r="AB13" t="inlineStr">
         <is>
-          <t>19h31m26.956s</t>
+          <t>19h31m34.421s</t>
         </is>
       </c>
       <c r="AC13" t="inlineStr">
         <is>
-          <t>+28°07'14.354"</t>
+          <t>+28°11'16.096"</t>
         </is>
       </c>
       <c r="AD13" t="n">
-        <v>5.11141169201572</v>
+        <v>5.111954529237394</v>
       </c>
       <c r="AE13" t="n">
-        <v>0.4907979967384806</v>
+        <v>0.4919699960473362</v>
       </c>
       <c r="AF13" t="n">
-        <v>0.0005369141006212885</v>
+        <v>292.8934835076952</v>
       </c>
       <c r="AG13" t="n">
-        <v>-0.001818579692375977</v>
+        <v>28.18764782500562</v>
       </c>
     </row>
     <row r="14">
@@ -2030,7 +2030,7 @@
         <v>-18.07</v>
       </c>
       <c r="J14" t="n">
-        <v>0.0002793596853207575</v>
+        <v>0.0002793596853207574</v>
       </c>
       <c r="K14" t="n">
         <v>403.990478515625</v>
@@ -2051,31 +2051,31 @@
         <v>15</v>
       </c>
       <c r="Q14" t="n">
-        <v>292.9978695154466</v>
+        <v>293.029063826663</v>
       </c>
       <c r="R14" t="n">
-        <v>27.88574503738063</v>
+        <v>27.95243382995252</v>
       </c>
       <c r="S14" t="inlineStr">
         <is>
-          <t>{'simbad': {'x': 0.777517557821191, 'y': 0.49270069959091145, 'z': 0.3907844263816014, 'ar': 5.109153573699976, 'dec': 0.4864730088287785, 'ar_deg': 292.7329366571904, 'dec_deg': 27.872850252919445, 'pmra': -2.52, 'pmdec': -4.776}, 'proper motion': {'ar': 5.109153259829807, 'dec': 0.4864724139700771, 'pmra': -2.52, 'pmdec': -4.776}, 'precession': {'x': 0.34511489879066815, 'y': -0.8133434324124187, 'z': 0.46836755607566627, 'ar': 5.11368040915581, 'dec': 0.48744224066181013, 'ang_zeta': 0.0028852121230277415, 'ang_theta': 0.002496113304495591, 'ang_z': 0.0028597582311986106}, 'nutation': {'x': 0.3451248237968405, 'y': -0.8133594764020093, 'z': 0.4683323799890944, 'ar': 5.113683656993178, 'dec': 0.4874024281287522, 'dpsi': 1.7724397752215108e-05, 'deps': 4.623967697805032e-05, 'epsm': 0.4090344953255741, 'w': -6.489953776770748}, 'aberration': {'x': 0.34515845048534766, 'y': -0.8133098214487507, 'z': 0.46839382830429727, 'ar': 5.113740646092717, 'dec': 0.48747197629627453, 'lambda_s': 2.9546338179558234, 'epsilon_m': 0.4090294332006951, 'omega_bar': 4.939647965644993}, 'refraction': {'x': 0.3453299660610592, 'y': -0.8136305322630063, 'z': 0.46770992239815135, 'ar': 5.1137775243732655, 'dec': 0.4866980652739612, 'R': -159.7720768437363, 'alt': -20.5893440791735}}</t>
+          <t>{'simbad': {'x': 0.777517557821191, 'y': 0.49270069959091145, 'z': 0.3907844263816014, 'ar': 5.109153573699976, 'dec': 0.4864730088287785, 'ar_deg': 292.7329366571904, 'dec_deg': 27.872850252919445, 'pmra': -2.52, 'pmdec': -4.776}, 'proper motion': {'ar': 5.1091532592946205, 'dec': 0.4864724129557713, 'pmra': -2.52, 'pmdec': -4.776}, 'precession': {'x': 0.3451208731960908, 'y': -0.8133400520184945, 'z': 0.46836902402584246, 'ar': 5.113688128381157, 'dec': 0.4874439021160266, 'ang_zeta': 0.0028901100151612243, 'ang_theta': 0.002500369232447987, 'ang_z': 0.0028646569776294853}, 'nutation': {'x': 0.34512938257468034, 'y': -0.8133566787755344, 'z': 0.46833387916619007, 'ar': 5.113689643505973, 'dec': 0.4874041248904035, 'dpsi': 1.519641027055965e-05, 'deps': 4.577484563030587e-05, 'epsm': 0.4090343959020549, 'w': -6.5047412493804675}, 'aberration': {'x': 0.34513928985978964, 'y': -0.813314044469435, 'z': 0.468400614499863, 'ar': 5.113718815388172, 'dec': 0.487479657176148, 'lambda_s': 3.229878486430863, 'epsilon_m': 0.40902933380891293, 'omega_bar': 4.939650435148504}, 'refraction': {'x': 0.3455596938406348, 'y': -0.8129408463285115, 'z': 0.4687383901105704, 'ar': 5.114321967811884, 'dec': 0.4878620042785203, 'R': 135.27397942142085, 'alt': 24.3142562394949}}</t>
         </is>
       </c>
       <c r="T14" t="inlineStr">
         <is>
-          <t>19h31m59.489s</t>
+          <t>19h32m6.975s</t>
         </is>
       </c>
       <c r="U14" t="inlineStr">
         <is>
-          <t>+27°53'8.682"</t>
+          <t>+27°57'8.762"</t>
         </is>
       </c>
       <c r="V14" t="n">
-        <v>5.113777524373265</v>
+        <v>5.114321967811884</v>
       </c>
       <c r="W14" t="n">
-        <v>0.4866980652739612</v>
+        <v>0.4878620042785202</v>
       </c>
       <c r="X14" t="inlineStr">
         <is>
@@ -2095,25 +2095,25 @@
       </c>
       <c r="AB14" t="inlineStr">
         <is>
-          <t>19h31m59.489s</t>
+          <t>19h32m6.975s</t>
         </is>
       </c>
       <c r="AC14" t="inlineStr">
         <is>
-          <t>+27°53'8.682"</t>
+          <t>+27°57'8.762"</t>
         </is>
       </c>
       <c r="AD14" t="n">
-        <v>5.113777524373265</v>
+        <v>5.114321967811884</v>
       </c>
       <c r="AE14" t="n">
-        <v>0.4866980652739612</v>
+        <v>0.4878620042785202</v>
       </c>
       <c r="AF14" t="n">
-        <v>-0.001936164331198142</v>
+        <v>293.0290707285757</v>
       </c>
       <c r="AG14" t="n">
-        <v>-0.00147064940829722</v>
+        <v>27.95239163036261</v>
       </c>
     </row>
     <row r="15">
@@ -2168,31 +2168,31 @@
         <v>16</v>
       </c>
       <c r="Q15" t="n">
-        <v>293.0635867921236</v>
+        <v>293.0947165243546</v>
       </c>
       <c r="R15" t="n">
-        <v>27.96456767618079</v>
+        <v>28.03131212271438</v>
       </c>
       <c r="S15" t="inlineStr">
         <is>
-          <t>{'simbad': {'x': 0.7658951968270207, 'y': 0.5593418314187893, 'z': 0.3170824231999841, 'ar': 5.110304807887032, 'dec': 0.48784888768862644, 'ar_deg': 292.7988975173399, 'dec_deg': 27.95168230471, 'pmra': -4.12, 'pmdec': -4.009}, 'proper motion': {'ar': 5.110304294734216, 'dec': 0.48784838836104394, 'pmra': -4.12, 'pmdec': -4.009}, 'precession': {'x': 0.3457948132443118, 'y': -0.8123519678216704, 'z': 0.4695851653423386, 'ar': 5.114827978154119, 'dec': 0.4888208578131763, 'ang_zeta': 0.0028852121230277415, 'ang_theta': 0.002496113304495591, 'ang_z': 0.0028597582311986106}, 'nutation': {'x': 0.3458047135435243, 'y': -0.8123680570576788, 'z': 0.4695500398928888, 'ar': 5.114831158312245, 'dec': 0.4887810734798783, 'dpsi': 1.7724397752215108e-05, 'deps': 4.623967697805032e-05, 'epsm': 0.4090344953255741, 'w': -6.489953776770748}, 'aberration': {'x': 0.3458383224557802, 'y': -0.8123182344790318, 'z': 0.4696114784093773, 'ar': 5.1148882872888635, 'dec': 0.488850661480278, 'lambda_s': 2.9546338179558234, 'epsilon_m': 0.4090294332006951, 'omega_bar': 4.939647965644993}, 'refraction': {'x': 0.3460105640004008, 'y': -0.8126411342452514, 'z': 0.46892544880046283, 'ar': 5.114924507226723, 'dec': 0.48807377984613426, 'R': -160.37908596988487, 'alt': -20.51300490115246}}</t>
+          <t>{'simbad': {'x': 0.7658951968270207, 'y': 0.5593418314187893, 'z': 0.3170824231999841, 'ar': 5.110304807887032, 'dec': 0.48784888768862644, 'ar_deg': 292.7988975173399, 'dec_deg': 27.95168230471, 'pmra': -4.12, 'pmdec': -4.009}, 'proper motion': {'ar': 5.110304293859229, 'dec': 0.4878483875096302, 'pmra': -4.12, 'pmdec': -4.009}, 'precession': {'x': 0.3458007724497421, 'y': -0.8123485808158603, 'z': 0.46958663632988856, 'ar': 5.1148356911310415, 'dec': 0.48882252392435716, 'ang_zeta': 0.0028901100151612243, 'ang_theta': 0.002500369232447987, 'ang_z': 0.0028646569776294853}, 'nutation': {'x': 0.34580926064516865, 'y': -0.8123652538305997, 'z': 0.46955154096306273, 'ar': 5.114837140553843, 'dec': 0.4887827736281256, 'dpsi': 1.519641027055965e-05, 'deps': 4.577484563030587e-05, 'epsm': 0.4090343959020549, 'w': -6.5047412493804675}, 'aberration': {'x': 0.34581916280698777, 'y': -0.81232245535053, 'z': 0.46961828666349836, 'ar': 5.114866447257903, 'dec': 0.4888583729706784, 'lambda_s': 3.229878486430863, 'epsilon_m': 0.40902933380891293, 'omega_bar': 4.939650435148504}, 'refraction': {'x': 0.34623752886761794, 'y': -0.8119499921097769, 'z': 0.46995402319437374, 'ar': 5.115467823549419, 'dec': 0.48923869019556676, 'R': 134.70182507447464, 'alt': 24.407327070084353}}</t>
         </is>
       </c>
       <c r="T15" t="inlineStr">
         <is>
-          <t>19h32m15.261s</t>
+          <t>19h32m22.732s</t>
         </is>
       </c>
       <c r="U15" t="inlineStr">
         <is>
-          <t>+27°57'52.444"</t>
+          <t>+28°01'52.724"</t>
         </is>
       </c>
       <c r="V15" t="n">
-        <v>5.114924507226724</v>
+        <v>5.115467823549419</v>
       </c>
       <c r="W15" t="n">
-        <v>0.4880737798461343</v>
+        <v>0.4892386901955668</v>
       </c>
       <c r="X15" t="inlineStr">
         <is>
@@ -2212,25 +2212,25 @@
       </c>
       <c r="AB15" t="inlineStr">
         <is>
-          <t>19h32m15.261s</t>
+          <t>19h32m22.732s</t>
         </is>
       </c>
       <c r="AC15" t="inlineStr">
         <is>
-          <t>+27°57'52.444"</t>
+          <t>+28°01'52.724"</t>
         </is>
       </c>
       <c r="AD15" t="n">
-        <v>5.114924507226724</v>
+        <v>5.115467823549419</v>
       </c>
       <c r="AE15" t="n">
-        <v>0.4880737798461343</v>
+        <v>0.4892386901955668</v>
       </c>
       <c r="AF15" t="n">
-        <v>-0.001843963464182252</v>
+        <v>293.0947229791874</v>
       </c>
       <c r="AG15" t="n">
-        <v>7.188155379722616e-05</v>
+        <v>28.03131274686904</v>
       </c>
     </row>
     <row r="16">
@@ -2285,31 +2285,31 @@
         <v>17</v>
       </c>
       <c r="Q16" t="n">
-        <v>292.9438249121852</v>
+        <v>292.9749964287569</v>
       </c>
       <c r="R16" t="n">
-        <v>27.95498538520556</v>
+        <v>28.02182143905106</v>
       </c>
       <c r="S16" t="inlineStr">
         <is>
-          <t>{'simbad': {'x': 0.8246476002172156, 'y': 0.46232269168428036, 'z': 0.3259049926125543, 'ar': 5.108213685730425, 'dec': 0.48768627101390477, 'ar_deg': 292.67908504332, 'dec_deg': 27.942365055569997, 'pmra': -2.922, 'pmdec': -4.483}, 'proper motion': {'ar': 5.10821332179049, 'dec': 0.4876857126488381, 'pmra': -2.922, 'pmdec': -4.483}, 'precession': {'x': 0.3441256198244492, 'y': -0.813145860469084, 'z': 0.4694372880187853, 'ar': 5.112736414474311, 'dec': 0.4886533723842878, 'ang_zeta': 0.0028852121230277415, 'ang_theta': 0.002496113304495591, 'ang_z': 0.0028597582311986106}, 'nutation': {'x': 0.3441355340768354, 'y': -0.8131619700105905, 'z': 0.4694021140921155, 'ar': 5.112739644183816, 'dec': 0.48861353669239344, 'dpsi': 1.7724397752215108e-05, 'deps': 4.623967697805032e-05, 'epsm': 0.4090344953255741, 'w': -6.489953776770748}, 'aberration': {'x': 0.34416909808183627, 'y': -0.8131122710333902, 'z': 0.4694635945634746, 'ar': 5.112796589141579, 'dec': 0.4886831660099981, 'lambda_s': 2.9546338179558234, 'epsilon_m': 0.4090294332006951, 'omega_bar': 4.939647965644993}, 'refraction': {'x': 0.3443417622666342, 'y': -0.813434811843479, 'z': 0.4687777273295657, 'ar': 5.112834268103421, 'dec': 0.48790653731873235, 'R': -160.33813819437984, 'alt': -20.518139846803614}}</t>
+          <t>{'simbad': {'x': 0.8246476002172156, 'y': 0.46232269168428036, 'z': 0.3259049926125543, 'ar': 5.108213685730425, 'dec': 0.48768627101390477, 'ar_deg': 292.67908504332, 'dec_deg': 27.942365055569997, 'pmra': -2.922, 'pmdec': -4.483}, 'proper motion': {'ar': 5.108213321169929, 'dec': 0.4876857116967583, 'pmra': -2.922, 'pmdec': -4.483}, 'precession': {'x': 0.3441315876608325, 'y': -0.8131424897700164, 'z': 0.46943875181396516, 'ar': 5.112744126698317, 'dec': 0.48865503020138346, 'ang_zeta': 0.0028901100151612243, 'ang_theta': 0.002500369232447987, 'ang_z': 0.0028646569776294853}, 'nutation': {'x': 0.3441400878195648, 'y': -0.8131591792870756, 'z': 0.46940361001670183, 'ar': 5.112745625395928, 'dec': 0.4886152308616945, 'dpsi': 1.519641027055965e-05, 'deps': 4.577484563030587e-05, 'epsm': 0.4090343959020549, 'w': -6.5047412493804675}, 'aberration': {'x': 0.3441499128360418, 'y': -0.8131164763894745, 'z': 0.4694703753368364, 'ar': 5.112774722676739, 'dec': 0.4886908456896574, 'lambda_s': 3.229878486430863, 'epsilon_m': 0.40902933380891293, 'omega_bar': 4.939650435148504}, 'refraction': {'x': 0.34457057718201056, 'y': -0.8127433445405858, 'z': 0.46980780458123383, 'ar': 5.113378313700437, 'dec': 0.48907304651737643, 'R': 135.26385821760857, 'alt': 24.315897029373378}}</t>
         </is>
       </c>
       <c r="T16" t="inlineStr">
         <is>
-          <t>19h31m46.518s</t>
+          <t>19h31m53.999s</t>
         </is>
       </c>
       <c r="U16" t="inlineStr">
         <is>
-          <t>+27°57'17.947"</t>
+          <t>+28°01'18.557"</t>
         </is>
       </c>
       <c r="V16" t="n">
-        <v>5.112834268103421</v>
+        <v>5.113378313700437</v>
       </c>
       <c r="W16" t="n">
-        <v>0.4879065373187323</v>
+        <v>0.4890730465173764</v>
       </c>
       <c r="X16" t="inlineStr">
         <is>
@@ -2329,25 +2329,25 @@
       </c>
       <c r="AB16" t="inlineStr">
         <is>
-          <t>19h31m46.518s</t>
+          <t>19h31m53.999s</t>
         </is>
       </c>
       <c r="AC16" t="inlineStr">
         <is>
-          <t>+27°57'17.947"</t>
+          <t>+28°01'18.557"</t>
         </is>
       </c>
       <c r="AD16" t="n">
-        <v>5.112834268103421</v>
+        <v>5.113378313700437</v>
       </c>
       <c r="AE16" t="n">
-        <v>0.4879065373187323</v>
+        <v>0.4890730465173764</v>
       </c>
       <c r="AF16" t="n">
-        <v>0.007467343527252979</v>
+        <v>292.975016540334</v>
       </c>
       <c r="AG16" t="n">
-        <v>0.0005480449182719838</v>
+        <v>28.02173649251796</v>
       </c>
     </row>
     <row r="17">
@@ -2402,31 +2402,31 @@
         <v>18</v>
       </c>
       <c r="Q17" t="n">
-        <v>292.8366458976371</v>
+        <v>292.8678506514986</v>
       </c>
       <c r="R17" t="n">
-        <v>27.95483453900924</v>
+        <v>28.02176558894969</v>
       </c>
       <c r="S17" t="inlineStr">
         <is>
-          <t>{'simbad': {'x': 0.8694148225537149, 'y': 0.37143602175460855, 'z': 0.32581152230546157, 'ar': 5.1063424438743725, 'dec': 0.4876879965612459, 'ar_deg': 292.57187078252, 'dec_deg': 27.942463922149997, 'pmra': 0.064, 'pmdec': -4.051}, 'proper motion': {'ar': 5.106342451845679, 'dec': 0.48768749200249395, 'pmra': 0.064, 'pmdec': -4.051}, 'precession': {'x': 0.34260340889753294, 'y': -0.813789673474818, 'z': 0.4694350557399169, 'ar': 5.110864586153423, 'dec': 0.48865084422597505, 'ang_zeta': 0.0028852121230277415, 'ang_theta': 0.002496113304495591, 'ang_z': 0.0028597582311986106}, 'nutation': {'x': 0.3426133336357284, 'y': -0.8138058076663761, 'z': 0.46939984131174395, 'ar': 5.110867855606884, 'dec': 0.4886109627188122, 'dpsi': 1.7724397752215108e-05, 'deps': 4.623967697805032e-05, 'epsm': 0.4090344953255741, 'w': -6.489953776770748}, 'aberration': {'x': 0.3426468521744683, 'y': -0.8137562076543693, 'z': 0.4694613607091717, 'ar': 5.110924640143397, 'dec': 0.48868063602735873, 'lambda_s': 2.9546338179558234, 'epsilon_m': 0.4090294332006951, 'omega_bar': 4.939647965644993}, 'refraction': {'x': 0.3428200068049105, 'y': -0.8140786605933048, 'z': 0.4687754017660173, 'ar': 5.110963641410514, 'dec': 0.4879039045559424, 'R': -160.36980923815062, 'alt': -20.514168038232476}}</t>
+          <t>{'simbad': {'x': 0.8694148225537149, 'y': 0.37143602175460855, 'z': 0.32581152230546157, 'ar': 5.1063424438743725, 'dec': 0.4876879965612459, 'ar_deg': 292.57187078252, 'dec_deg': 27.942463922149997, 'pmra': 0.064, 'pmdec': -4.051}, 'proper motion': {'ar': 5.106342451859271, 'dec': 0.48768749114216037, 'pmra': 0.064, 'pmdec': -4.051}, 'precession': {'x': 0.34260938354865855, 'y': -0.813786317430017, 'z': 0.469436513138997, 'ar': 5.110872297377256, 'dec': 0.4886524947969642, 'ang_zeta': 0.0028901100151612243, 'ang_theta': 0.002500369232447987, 'ang_z': 0.0028646569776294853}, 'nutation': {'x': 0.3426178926978489, 'y': -0.8138030280672104, 'z': 0.4694013326695231, 'ar': 5.110873835778364, 'dec': 0.4886126517137847, 'dpsi': 1.519641027055965e-05, 'deps': 4.577484563030587e-05, 'epsm': 0.4090343959020549, 'w': -6.5047412493804675}, 'aberration': {'x': 0.3426276429198928, 'y': -0.813760397575207, 'z': 0.4694681178156822, 'ar': 5.110902747825847, 'dec': 0.4886882888923757, 'lambda_s': 3.229878486430863, 'epsilon_m': 0.40902933380891293, 'omega_bar': 4.939650435148504}, 'refraction': {'x': 0.34305028561517986, 'y': -0.8133867080471391, 'z': 0.4698069440861654, 'ar': 5.11150826710767, 'dec': 0.4890720717492202, 'R': 135.73947745305344, 'alt': 24.239009102664408}}</t>
         </is>
       </c>
       <c r="T17" t="inlineStr">
         <is>
-          <t>19h31m20.795s</t>
+          <t>19h31m28.284s</t>
         </is>
       </c>
       <c r="U17" t="inlineStr">
         <is>
-          <t>+27°57'17.404"</t>
+          <t>+28°01'18.356"</t>
         </is>
       </c>
       <c r="V17" t="n">
-        <v>5.110963641410514</v>
+        <v>5.111508267107671</v>
       </c>
       <c r="W17" t="n">
-        <v>0.4879039045559424</v>
+        <v>0.4890720717492201</v>
       </c>
       <c r="X17" t="inlineStr">
         <is>
@@ -2446,25 +2446,25 @@
       </c>
       <c r="AB17" t="inlineStr">
         <is>
-          <t>19h31m20.795s</t>
+          <t>19h31m28.284s</t>
         </is>
       </c>
       <c r="AC17" t="inlineStr">
         <is>
-          <t>+27°57'17.404"</t>
+          <t>+28°01'18.356"</t>
         </is>
       </c>
       <c r="AD17" t="n">
-        <v>5.110963641410514</v>
+        <v>5.111508267107671</v>
       </c>
       <c r="AE17" t="n">
-        <v>0.4879039045559424</v>
+        <v>0.4890720717492201</v>
       </c>
       <c r="AF17" t="n">
-        <v>-0.00107928828350623</v>
+        <v>292.8678797189532</v>
       </c>
       <c r="AG17" t="n">
-        <v>0.001911061748252507</v>
+        <v>28.02161438695228</v>
       </c>
     </row>
     <row r="18">
@@ -2498,7 +2498,7 @@
         <v>2.46</v>
       </c>
       <c r="J18" t="n">
-        <v>0.008543152790713068</v>
+        <v>0.008543152790710273</v>
       </c>
       <c r="K18" t="n">
         <v>683.22802734375</v>
@@ -2519,31 +2519,31 @@
         <v>22</v>
       </c>
       <c r="Q18" t="n">
-        <v>293.0635867921236</v>
+        <v>293.0947165243546</v>
       </c>
       <c r="R18" t="n">
-        <v>27.96456767618079</v>
+        <v>28.03131212271438</v>
       </c>
       <c r="S18" t="inlineStr">
         <is>
-          <t>{'simbad': {'x': 0.7658951968270207, 'y': 0.5593418314187893, 'z': 0.3170824231999841, 'ar': 5.110304807887032, 'dec': 0.48784888768862644, 'ar_deg': 292.7988975173399, 'dec_deg': 27.95168230471, 'pmra': -4.12, 'pmdec': -4.009}, 'proper motion': {'ar': 5.110304294734216, 'dec': 0.48784838836104394, 'pmra': -4.12, 'pmdec': -4.009}, 'precession': {'x': 0.3457948132443118, 'y': -0.8123519678216704, 'z': 0.4695851653423386, 'ar': 5.114827978154119, 'dec': 0.4888208578131763, 'ang_zeta': 0.0028852121230277415, 'ang_theta': 0.002496113304495591, 'ang_z': 0.0028597582311986106}, 'nutation': {'x': 0.3458047135435243, 'y': -0.8123680570576788, 'z': 0.4695500398928888, 'ar': 5.114831158312245, 'dec': 0.4887810734798783, 'dpsi': 1.7724397752215108e-05, 'deps': 4.623967697805032e-05, 'epsm': 0.4090344953255741, 'w': -6.489953776770748}, 'aberration': {'x': 0.3458383224557802, 'y': -0.8123182344790318, 'z': 0.4696114784093773, 'ar': 5.1148882872888635, 'dec': 0.488850661480278, 'lambda_s': 2.9546338179558234, 'epsilon_m': 0.4090294332006951, 'omega_bar': 4.939647965644993}, 'refraction': {'x': 0.3460105640004008, 'y': -0.8126411342452514, 'z': 0.46892544880046283, 'ar': 5.114924507226723, 'dec': 0.48807377984613426, 'R': -160.37908596988487, 'alt': -20.51300490115246}}</t>
+          <t>{'simbad': {'x': 0.7658951968270207, 'y': 0.5593418314187893, 'z': 0.3170824231999841, 'ar': 5.110304807887032, 'dec': 0.48784888768862644, 'ar_deg': 292.7988975173399, 'dec_deg': 27.95168230471, 'pmra': -4.12, 'pmdec': -4.009}, 'proper motion': {'ar': 5.110304293859229, 'dec': 0.4878483875096302, 'pmra': -4.12, 'pmdec': -4.009}, 'precession': {'x': 0.3458007724497421, 'y': -0.8123485808158603, 'z': 0.46958663632988856, 'ar': 5.1148356911310415, 'dec': 0.48882252392435716, 'ang_zeta': 0.0028901100151612243, 'ang_theta': 0.002500369232447987, 'ang_z': 0.0028646569776294853}, 'nutation': {'x': 0.34580926064516865, 'y': -0.8123652538305997, 'z': 0.46955154096306273, 'ar': 5.114837140553843, 'dec': 0.4887827736281256, 'dpsi': 1.519641027055965e-05, 'deps': 4.577484563030587e-05, 'epsm': 0.4090343959020549, 'w': -6.5047412493804675}, 'aberration': {'x': 0.34581916280698777, 'y': -0.81232245535053, 'z': 0.46961828666349836, 'ar': 5.114866447257903, 'dec': 0.4888583729706784, 'lambda_s': 3.229878486430863, 'epsilon_m': 0.40902933380891293, 'omega_bar': 4.939650435148504}, 'refraction': {'x': 0.34623752886761794, 'y': -0.8119499921097769, 'z': 0.46995402319437374, 'ar': 5.115467823549419, 'dec': 0.48923869019556676, 'R': 134.70182507447464, 'alt': 24.407327070084353}}</t>
         </is>
       </c>
       <c r="T18" t="inlineStr">
         <is>
-          <t>19h32m15.261s</t>
+          <t>19h32m22.732s</t>
         </is>
       </c>
       <c r="U18" t="inlineStr">
         <is>
-          <t>+27°57'52.444"</t>
+          <t>+28°01'52.724"</t>
         </is>
       </c>
       <c r="V18" t="n">
-        <v>5.114924507226724</v>
+        <v>5.115467823549419</v>
       </c>
       <c r="W18" t="n">
-        <v>0.4880737798461343</v>
+        <v>0.4892386901955668</v>
       </c>
       <c r="X18" t="inlineStr">
         <is>
@@ -2563,25 +2563,25 @@
       </c>
       <c r="AB18" t="inlineStr">
         <is>
-          <t>19h32m15.261s</t>
+          <t>19h32m22.732s</t>
         </is>
       </c>
       <c r="AC18" t="inlineStr">
         <is>
-          <t>+27°57'52.444"</t>
+          <t>+28°01'52.724"</t>
         </is>
       </c>
       <c r="AD18" t="n">
-        <v>5.114924507226724</v>
+        <v>5.115467823549419</v>
       </c>
       <c r="AE18" t="n">
-        <v>0.4880737798461343</v>
+        <v>0.4892386901955668</v>
       </c>
       <c r="AF18" t="n">
-        <v>0.002784345697079971</v>
+        <v>293.0947232054796</v>
       </c>
       <c r="AG18" t="n">
-        <v>0.007241571822135029</v>
+        <v>28.0313084394361</v>
       </c>
     </row>
     <row r="19">
@@ -2636,31 +2636,31 @@
         <v>29</v>
       </c>
       <c r="Q19" t="n">
-        <v>293.0439813971735</v>
+        <v>293.0752106168623</v>
       </c>
       <c r="R19" t="n">
-        <v>27.79906294046827</v>
+        <v>27.86558780443116</v>
       </c>
       <c r="S19" t="inlineStr">
         <is>
-          <t>{'simbad': {'x': 0.7234418187578643, 'y': 0.5063524164086586, 'z': 0.46929645776356116, 'ar': 5.109953865505049, 'dec': 0.48495439343234115, 'ar_deg': 292.77879, 'dec_deg': 27.785839999999997, 'pmra': nan, 'pmdec': nan}, 'proper motion': {'ar': 5.109953865505049, 'dec': 0.48495439343234115, 'pmra': 0, 'pmdec': 0}, 'precession': {'x': 0.3460474291124171, 'y': -0.8137177389838324, 'z': 0.4670274275326089, 'ar': 5.1144858900849055, 'dec': 0.48592606681350337, 'ang_zeta': 0.0028852121230277415, 'ang_theta': 0.002496113304495591, 'ang_z': 0.0028597582311986106}, 'nutation': {'x': 0.3460573696526204, 'y': -0.8137337058410687, 'z': 0.4669922407142014, 'ar': 5.114489168634659, 'dec': 0.4858862740693912, 'dpsi': 1.7724397752215108e-05, 'deps': 4.623967697805032e-05, 'epsm': 0.4090344953255741, 'w': -6.489953776770748}, 'aberration': {'x': 0.34609106575415866, 'y': -0.8136841256470773, 'z': 0.4670536563127431, 'ar': 5.114546180835829, 'dec': 0.485955729463534, 'lambda_s': 2.9546338179558234, 'epsilon_m': 0.4090294332006951, 'omega_bar': 4.939647965644993}, 'refraction': {'x': 0.34626124974192063, 'y': -0.8140025448568311, 'z': 0.4663721731554807, 'ar': 5.1145823285336895, 'dec': 0.48518517728030774, 'R': -159.07452989666425, 'alt': -20.677653064930396}}</t>
+          <t>{'simbad': {'x': 0.7234418187578643, 'y': 0.5063524164086586, 'z': 0.46929645776356116, 'ar': 5.109953865505049, 'dec': 0.48495439343234115, 'ar_deg': 292.77879, 'dec_deg': 27.785839999999997, 'pmra': nan, 'pmdec': nan}, 'proper motion': {'ar': 5.109953865505049, 'dec': 0.48495439343234115, 'pmra': 0, 'pmdec': 0}, 'precession': {'x': 0.3460534131355237, 'y': -0.8137143488326647, 'z': 0.46702890034888306, 'ar': 5.114493618153882, 'dec': 0.48592773243845666, 'ang_zeta': 0.0028901100151612243, 'ang_theta': 0.002500369232447987, 'ang_z': 0.0028646569776294853}, 'nutation': {'x': 0.3460619358324142, 'y': -0.8137309012433176, 'z': 0.4669937439941352, 'ar': 5.114495161857544, 'dec': 0.48588797411033613, 'dpsi': 1.519641027055965e-05, 'deps': 4.577484563030587e-05, 'epsm': 0.4090343959020549, 'w': -6.5047412493804675}, 'aberration': {'x': 0.3460719311837043, 'y': -0.8136883671114326, 'z': 0.4670604454182688, 'ar': 5.114524389877057, 'dec': 0.48596340747395483, 'lambda_s': 3.229878486430863, 'epsilon_m': 0.40902933380891293, 'omega_bar': 4.939650435148504}, 'refraction': {'x': 0.34649240608083376, 'y': -0.8133149747956382, 'z': 0.4673989348527492, 'ar': 5.115127381240089, 'dec': 0.4863462551909015, 'R': 135.3820235584077, 'alt': 24.296753280144568}}</t>
         </is>
       </c>
       <c r="T19" t="inlineStr">
         <is>
-          <t>19h32m10.556s</t>
+          <t>19h32m18.051s</t>
         </is>
       </c>
       <c r="U19" t="inlineStr">
         <is>
-          <t>+27°47'56.627"</t>
+          <t>+27°51'56.116"</t>
         </is>
       </c>
       <c r="V19" t="n">
-        <v>5.11458232853369</v>
+        <v>5.115127381240089</v>
       </c>
       <c r="W19" t="n">
-        <v>0.4851851772803078</v>
+        <v>0.4863462551909015</v>
       </c>
       <c r="X19" t="inlineStr">
         <is>
@@ -2680,25 +2680,25 @@
       </c>
       <c r="AB19" t="inlineStr">
         <is>
-          <t>19h32m10.556s</t>
+          <t>19h32m18.051s</t>
         </is>
       </c>
       <c r="AC19" t="inlineStr">
         <is>
-          <t>+27°47'56.627"</t>
+          <t>+27°51'56.116"</t>
         </is>
       </c>
       <c r="AD19" t="n">
-        <v>5.11458232853369</v>
+        <v>5.115127381240089</v>
       </c>
       <c r="AE19" t="n">
-        <v>0.4851851772803078</v>
+        <v>0.4863462551909015</v>
       </c>
       <c r="AF19" t="n">
-        <v>-0.0008769879170245076</v>
+        <v>293.0752099314029</v>
       </c>
       <c r="AG19" t="n">
-        <v>0.007168134826116557</v>
+        <v>27.8655720384382</v>
       </c>
     </row>
   </sheetData>

</xml_diff>